<commit_message>
Updates of local parameter files
</commit_message>
<xml_diff>
--- a/03_Codebase/res/experiments_config/model_params.xlsx
+++ b/03_Codebase/res/experiments_config/model_params.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mAx/Documents/Master/04/Master_Thesis/03_Codebase/res/experiments_config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B049EB5E-AC57-8444-9FD9-8A3537D1F048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F53692-03AF-CD40-B1C9-41532BA0C695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18420" yWindow="7640" windowWidth="28240" windowHeight="17240" xr2:uid="{98D784FE-0FB7-BA4F-BB15-23B304B85074}"/>
+    <workbookView xWindow="-31060" yWindow="7680" windowWidth="28240" windowHeight="17240" xr2:uid="{98D784FE-0FB7-BA4F-BB15-23B304B85074}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
   <si>
     <t>model</t>
   </si>
@@ -47,21 +47,9 @@
     <t>temperature</t>
   </si>
   <si>
-    <t>top_p</t>
-  </si>
-  <si>
-    <t>gpt-3.5-turbo</t>
-  </si>
-  <si>
-    <t>gpt-4</t>
-  </si>
-  <si>
     <t>gpt-4o</t>
   </si>
   <si>
-    <t>llama2</t>
-  </si>
-  <si>
     <t>llama3</t>
   </si>
   <si>
@@ -75,6 +63,30 @@
   </si>
   <si>
     <t>model_id</t>
+  </si>
+  <si>
+    <t>gemma2:27b</t>
+  </si>
+  <si>
+    <t>gpt-4o-mini</t>
+  </si>
+  <si>
+    <t>phi3</t>
+  </si>
+  <si>
+    <t>phi3:medium</t>
+  </si>
+  <si>
+    <t>system</t>
+  </si>
+  <si>
+    <t>Linux</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>llama3:70b</t>
   </si>
 </sst>
 </file>
@@ -446,17 +458,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{061A15C7-5A39-BE49-968A-8B9EB1E3B441}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -468,7 +487,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -476,101 +495,135 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>0.7</v>
+        <v>0.7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>0.7</v>
+        <v>0.7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
       <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>0.7</v>
+        <v>0.7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>0.7</v>
+        <v>0.7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>0.7</v>
+        <v>0.7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>0.7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>0.7</v>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>0.7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>0.7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>